<commit_message>
Did a lot of enhancement and improvements especially to the organization, also did critical changes to the REFramework structure, in addition to some error and exception handling
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29628"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\omarf\Documents\UiPath\AddStudent\Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Personal\Work\UiPath\Projects\AddStudent-Automation-main\AddStudent_Automation\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C7424DDD-5162-4B68-9A83-D3F0AFAB2CD4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3F277A97-8506-4560-9B97-9021684F578A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="22932" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="53">
   <si>
     <t>Name</t>
   </si>
@@ -181,6 +181,9 @@
   </si>
   <si>
     <t>Email</t>
+  </si>
+  <si>
+    <t>CMDPath</t>
   </si>
 </sst>
 </file>
@@ -562,12 +565,12 @@
       <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="43.5546875" customWidth="1"/>
+    <col min="1" max="1" width="43.54296875" customWidth="1"/>
     <col min="2" max="2" width="43" customWidth="1"/>
-    <col min="3" max="3" width="81.44140625" customWidth="1"/>
-    <col min="4" max="26" width="8.6640625" customWidth="1"/>
+    <col min="3" max="3" width="81.453125" customWidth="1"/>
+    <col min="4" max="26" width="8.6328125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="14.25" customHeight="1">
@@ -615,7 +618,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="3" spans="1:26" ht="43.2">
+    <row r="3" spans="1:26" ht="43.5">
       <c r="A3" s="2" t="s">
         <v>31</v>
       </c>
@@ -627,7 +630,7 @@
       </c>
     </row>
     <row r="4" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="5" spans="1:26" ht="28.8">
+    <row r="5" spans="1:26" ht="29">
       <c r="A5" t="s">
         <v>20</v>
       </c>
@@ -1646,12 +1649,12 @@
       <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="41" customWidth="1"/>
     <col min="2" max="2" width="51" customWidth="1"/>
-    <col min="3" max="3" width="75.44140625" customWidth="1"/>
-    <col min="4" max="26" width="8.6640625" customWidth="1"/>
+    <col min="3" max="3" width="75.453125" customWidth="1"/>
+    <col min="4" max="26" width="8.6328125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="14.25" customHeight="1">
@@ -1688,7 +1691,7 @@
       <c r="Y1" s="1"/>
       <c r="Z1" s="1"/>
     </row>
-    <row r="2" spans="1:26" ht="28.8">
+    <row r="2" spans="1:26" ht="29">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -1699,7 +1702,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="3" spans="1:26" ht="43.2">
+    <row r="3" spans="1:26" ht="43.5">
       <c r="A3" t="s">
         <v>33</v>
       </c>
@@ -1813,7 +1816,7 @@
       </c>
     </row>
     <row r="16" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="17" spans="1:3" ht="28.8">
+    <row r="17" spans="1:3" ht="29">
       <c r="A17" t="s">
         <v>40</v>
       </c>
@@ -2806,15 +2809,15 @@
   <dimension ref="A1:Z1000"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="31.88671875" customWidth="1"/>
-    <col min="2" max="2" width="30.109375" customWidth="1"/>
-    <col min="3" max="3" width="60.33203125" customWidth="1"/>
-    <col min="4" max="26" width="65.44140625" customWidth="1"/>
+    <col min="1" max="1" width="31.90625" customWidth="1"/>
+    <col min="2" max="2" width="30.08984375" customWidth="1"/>
+    <col min="3" max="3" width="60.36328125" customWidth="1"/>
+    <col min="4" max="26" width="65.453125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="14.25" customHeight="1">
@@ -2890,7 +2893,17 @@
         <v>47</v>
       </c>
     </row>
-    <row r="5" spans="1:26" ht="14.25" customHeight="1"/>
+    <row r="5" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A5" t="s">
+        <v>52</v>
+      </c>
+      <c r="B5" t="s">
+        <v>52</v>
+      </c>
+      <c r="C5" t="s">
+        <v>47</v>
+      </c>
+    </row>
     <row r="6" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="7" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="8" spans="1:26" ht="14.25" customHeight="1"/>

</xml_diff>

<commit_message>
Critical and huge changes in the core of the project, now you can choose one of the playlists you have
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Personal\Work\UiPath\Projects\AddStudent-Automation-main\AddStudent_Automation\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3F277A97-8506-4560-9B97-9021684F578A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{440F5B4A-6CB4-4D65-89D3-608A59F57093}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="55">
   <si>
     <t>Name</t>
   </si>
@@ -184,6 +184,12 @@
   </si>
   <si>
     <t>CMDPath</t>
+  </si>
+  <si>
+    <t>Playlists</t>
+  </si>
+  <si>
+    <t>Playlist</t>
   </si>
 </sst>
 </file>
@@ -2904,7 +2910,17 @@
         <v>47</v>
       </c>
     </row>
-    <row r="6" spans="1:26" ht="14.25" customHeight="1"/>
+    <row r="6" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A6" t="s">
+        <v>53</v>
+      </c>
+      <c r="B6" t="s">
+        <v>54</v>
+      </c>
+      <c r="C6" t="s">
+        <v>47</v>
+      </c>
+    </row>
     <row r="7" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="8" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="9" spans="1:26" ht="14.25" customHeight="1"/>

</xml_diff>